<commit_message>
Added filling user's dayoffs, added convenient main function, added some comments, added more filling table(count of workdays), reworked file saving
</commit_message>
<xml_diff>
--- a/flask-app/project/xlsx-table/template.xlsx
+++ b/flask-app/project/xlsx-table/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pomid\Documents\GitHub\PythonTermTask\flask-app\project\xlsx-table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F515A6A-A097-44FC-939C-45AB30A41D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA928E29-A538-4FCA-8AD5-26178D103F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="431" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -621,9 +621,57 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="26" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -642,130 +690,82 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="26" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="26" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1189,7 +1189,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1231,7 +1231,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -1255,7 +1255,7 @@
   <dimension ref="A1:BM28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="AK17" sqref="AK17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -1280,117 +1280,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="AN1" s="90" t="s">
+      <c r="AN1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="AO1" s="90"/>
-      <c r="AP1" s="90"/>
+      <c r="AO1" s="69"/>
+      <c r="AP1" s="69"/>
     </row>
     <row r="2" spans="1:43" x14ac:dyDescent="0.3">
-      <c r="AJ2" s="93" t="s">
+      <c r="AJ2" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="AK2" s="93"/>
-      <c r="AL2" s="93"/>
-      <c r="AM2" s="93"/>
-      <c r="AN2" s="90">
+      <c r="AK2" s="70"/>
+      <c r="AL2" s="70"/>
+      <c r="AM2" s="70"/>
+      <c r="AN2" s="69">
         <v>301008</v>
       </c>
-      <c r="AO2" s="90"/>
-      <c r="AP2" s="90"/>
+      <c r="AO2" s="69"/>
+      <c r="AP2" s="69"/>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B3" s="62"/>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91"/>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="91"/>
-      <c r="N3" s="91"/>
-      <c r="O3" s="91"/>
-      <c r="P3" s="91"/>
-      <c r="Q3" s="91"/>
-      <c r="R3" s="91"/>
-      <c r="S3" s="91"/>
-      <c r="T3" s="91"/>
-      <c r="U3" s="91"/>
-      <c r="V3" s="91"/>
-      <c r="W3" s="91"/>
-      <c r="X3" s="91"/>
-      <c r="Y3" s="91"/>
-      <c r="Z3" s="91"/>
-      <c r="AA3" s="91"/>
-      <c r="AB3" s="91"/>
-      <c r="AC3" s="91"/>
-      <c r="AD3" s="91"/>
-      <c r="AE3" s="91"/>
-      <c r="AF3" s="91"/>
-      <c r="AG3" s="91"/>
-      <c r="AH3" s="91"/>
-      <c r="AI3" s="91"/>
-      <c r="AJ3" s="69" t="s">
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
+      <c r="O3" s="71"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="71"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="71"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="71"/>
+      <c r="W3" s="71"/>
+      <c r="X3" s="71"/>
+      <c r="Y3" s="71"/>
+      <c r="Z3" s="71"/>
+      <c r="AA3" s="71"/>
+      <c r="AB3" s="71"/>
+      <c r="AC3" s="71"/>
+      <c r="AD3" s="71"/>
+      <c r="AE3" s="71"/>
+      <c r="AF3" s="71"/>
+      <c r="AG3" s="71"/>
+      <c r="AH3" s="71"/>
+      <c r="AI3" s="71"/>
+      <c r="AJ3" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="AK3" s="69"/>
-      <c r="AL3" s="69"/>
-      <c r="AN3" s="90"/>
-      <c r="AO3" s="90"/>
-      <c r="AP3" s="90"/>
+      <c r="AK3" s="72"/>
+      <c r="AL3" s="72"/>
+      <c r="AN3" s="69"/>
+      <c r="AO3" s="69"/>
+      <c r="AP3" s="69"/>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.3">
       <c r="AM4" s="62"/>
-      <c r="AN4" s="90"/>
-      <c r="AO4" s="90"/>
-      <c r="AP4" s="90"/>
+      <c r="AN4" s="69"/>
+      <c r="AO4" s="69"/>
+      <c r="AP4" s="69"/>
     </row>
     <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B5" s="62"/>
-      <c r="C5" s="91" t="s">
+      <c r="C5" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
-      <c r="L5" s="91"/>
-      <c r="M5" s="91"/>
-      <c r="N5" s="91"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="91"/>
-      <c r="S5" s="91"/>
-      <c r="T5" s="91"/>
-      <c r="U5" s="91"/>
-      <c r="V5" s="91"/>
-      <c r="W5" s="91"/>
-      <c r="X5" s="91"/>
-      <c r="Y5" s="91"/>
-      <c r="Z5" s="91"/>
-      <c r="AA5" s="91"/>
-      <c r="AB5" s="91"/>
-      <c r="AC5" s="91"/>
-      <c r="AD5" s="91"/>
-      <c r="AE5" s="91"/>
-      <c r="AF5" s="91"/>
-      <c r="AG5" s="91"/>
-      <c r="AH5" s="91"/>
-      <c r="AI5" s="91"/>
-      <c r="AJ5" s="91"/>
-      <c r="AK5" s="91"/>
-      <c r="AL5" s="91"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="71"/>
+      <c r="O5" s="71"/>
+      <c r="P5" s="71"/>
+      <c r="Q5" s="71"/>
+      <c r="R5" s="71"/>
+      <c r="S5" s="71"/>
+      <c r="T5" s="71"/>
+      <c r="U5" s="71"/>
+      <c r="V5" s="71"/>
+      <c r="W5" s="71"/>
+      <c r="X5" s="71"/>
+      <c r="Y5" s="71"/>
+      <c r="Z5" s="71"/>
+      <c r="AA5" s="71"/>
+      <c r="AB5" s="71"/>
+      <c r="AC5" s="71"/>
+      <c r="AD5" s="71"/>
+      <c r="AE5" s="71"/>
+      <c r="AF5" s="71"/>
+      <c r="AG5" s="71"/>
+      <c r="AH5" s="71"/>
+      <c r="AI5" s="71"/>
+      <c r="AJ5" s="71"/>
+      <c r="AK5" s="71"/>
+      <c r="AL5" s="71"/>
       <c r="AM5" s="62"/>
       <c r="AN5" s="60"/>
       <c r="AO5" s="60"/>
@@ -1398,99 +1398,99 @@
     </row>
     <row r="6" spans="1:43" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="T7" s="92" t="s">
+      <c r="T7" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="U7" s="92"/>
-      <c r="V7" s="92"/>
-      <c r="W7" s="92"/>
-      <c r="X7" s="92"/>
-      <c r="Y7" s="92" t="s">
+      <c r="U7" s="73"/>
+      <c r="V7" s="73"/>
+      <c r="W7" s="73"/>
+      <c r="X7" s="73"/>
+      <c r="Y7" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="Z7" s="92"/>
-      <c r="AA7" s="92"/>
-      <c r="AB7" s="92"/>
-      <c r="AC7" s="92"/>
-      <c r="AF7" s="92" t="s">
+      <c r="Z7" s="73"/>
+      <c r="AA7" s="73"/>
+      <c r="AB7" s="73"/>
+      <c r="AC7" s="73"/>
+      <c r="AF7" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="AG7" s="92"/>
-      <c r="AH7" s="92"/>
-      <c r="AI7" s="92"/>
-      <c r="AJ7" s="92"/>
-      <c r="AK7" s="92"/>
+      <c r="AG7" s="73"/>
+      <c r="AH7" s="73"/>
+      <c r="AI7" s="73"/>
+      <c r="AJ7" s="73"/>
+      <c r="AK7" s="73"/>
     </row>
     <row r="8" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="T8" s="92"/>
-      <c r="U8" s="92"/>
-      <c r="V8" s="92"/>
-      <c r="W8" s="92"/>
-      <c r="X8" s="92"/>
-      <c r="Y8" s="92"/>
-      <c r="Z8" s="92"/>
-      <c r="AA8" s="92"/>
-      <c r="AB8" s="92"/>
-      <c r="AC8" s="92"/>
-      <c r="AF8" s="70" t="s">
+      <c r="T8" s="73"/>
+      <c r="U8" s="73"/>
+      <c r="V8" s="73"/>
+      <c r="W8" s="73"/>
+      <c r="X8" s="73"/>
+      <c r="Y8" s="73"/>
+      <c r="Z8" s="73"/>
+      <c r="AA8" s="73"/>
+      <c r="AB8" s="73"/>
+      <c r="AC8" s="73"/>
+      <c r="AF8" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="AG8" s="71"/>
-      <c r="AH8" s="72"/>
-      <c r="AI8" s="70" t="s">
+      <c r="AG8" s="87"/>
+      <c r="AH8" s="88"/>
+      <c r="AI8" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="AJ8" s="71"/>
-      <c r="AK8" s="72"/>
+      <c r="AJ8" s="87"/>
+      <c r="AK8" s="88"/>
     </row>
     <row r="9" spans="1:43" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="82"/>
-      <c r="I9" s="82"/>
-      <c r="J9" s="82"/>
-      <c r="K9" s="82"/>
-      <c r="L9" s="82"/>
-      <c r="M9" s="82"/>
-      <c r="N9" s="82"/>
-      <c r="O9" s="82"/>
-      <c r="P9" s="82"/>
-      <c r="Q9" s="82"/>
-      <c r="R9" s="82"/>
-      <c r="S9" s="82"/>
-      <c r="T9" s="83"/>
-      <c r="U9" s="83"/>
-      <c r="V9" s="83"/>
-      <c r="W9" s="83"/>
-      <c r="X9" s="83"/>
-      <c r="Y9" s="73">
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="92"/>
+      <c r="L9" s="92"/>
+      <c r="M9" s="92"/>
+      <c r="N9" s="92"/>
+      <c r="O9" s="92"/>
+      <c r="P9" s="92"/>
+      <c r="Q9" s="92"/>
+      <c r="R9" s="92"/>
+      <c r="S9" s="92"/>
+      <c r="T9" s="93"/>
+      <c r="U9" s="93"/>
+      <c r="V9" s="93"/>
+      <c r="W9" s="93"/>
+      <c r="X9" s="93"/>
+      <c r="Y9" s="89">
         <f>AF9+15</f>
         <v>44090</v>
       </c>
-      <c r="Z9" s="74"/>
-      <c r="AA9" s="74"/>
-      <c r="AB9" s="74"/>
-      <c r="AC9" s="75"/>
-      <c r="AF9" s="73">
+      <c r="Z9" s="90"/>
+      <c r="AA9" s="90"/>
+      <c r="AB9" s="90"/>
+      <c r="AC9" s="91"/>
+      <c r="AF9" s="89">
         <v>44075</v>
       </c>
-      <c r="AG9" s="74"/>
-      <c r="AH9" s="75"/>
-      <c r="AI9" s="73">
+      <c r="AG9" s="90"/>
+      <c r="AH9" s="91"/>
+      <c r="AI9" s="89">
         <f>AF9+30</f>
         <v>44105</v>
       </c>
-      <c r="AJ9" s="74"/>
-      <c r="AK9" s="75"/>
+      <c r="AJ9" s="90"/>
+      <c r="AK9" s="91"/>
     </row>
     <row r="12" spans="1:43" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="84" t="s">
+      <c r="A12" s="74" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="76" t="s">
@@ -1499,42 +1499,42 @@
       <c r="C12" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="86" t="s">
+      <c r="D12" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="88" t="s">
+      <c r="E12" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="88"/>
-      <c r="J12" s="88"/>
-      <c r="K12" s="88"/>
-      <c r="L12" s="88"/>
-      <c r="M12" s="88"/>
-      <c r="N12" s="88"/>
-      <c r="O12" s="88"/>
-      <c r="P12" s="88"/>
-      <c r="Q12" s="88"/>
-      <c r="R12" s="88"/>
-      <c r="S12" s="88"/>
-      <c r="T12" s="88"/>
-      <c r="U12" s="88"/>
-      <c r="V12" s="88"/>
-      <c r="W12" s="88"/>
-      <c r="X12" s="88"/>
-      <c r="Y12" s="88"/>
-      <c r="Z12" s="88"/>
-      <c r="AA12" s="88"/>
-      <c r="AB12" s="88"/>
-      <c r="AC12" s="88"/>
-      <c r="AD12" s="88"/>
-      <c r="AE12" s="88"/>
-      <c r="AF12" s="88"/>
-      <c r="AG12" s="88"/>
-      <c r="AH12" s="88"/>
-      <c r="AI12" s="88"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="80"/>
+      <c r="H12" s="80"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="80"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="80"/>
+      <c r="M12" s="80"/>
+      <c r="N12" s="80"/>
+      <c r="O12" s="80"/>
+      <c r="P12" s="80"/>
+      <c r="Q12" s="80"/>
+      <c r="R12" s="80"/>
+      <c r="S12" s="80"/>
+      <c r="T12" s="80"/>
+      <c r="U12" s="80"/>
+      <c r="V12" s="80"/>
+      <c r="W12" s="80"/>
+      <c r="X12" s="80"/>
+      <c r="Y12" s="80"/>
+      <c r="Z12" s="80"/>
+      <c r="AA12" s="80"/>
+      <c r="AB12" s="80"/>
+      <c r="AC12" s="80"/>
+      <c r="AD12" s="80"/>
+      <c r="AE12" s="80"/>
+      <c r="AF12" s="80"/>
+      <c r="AG12" s="80"/>
+      <c r="AH12" s="80"/>
+      <c r="AI12" s="80"/>
       <c r="AJ12" s="76" t="s">
         <v>18</v>
       </c>
@@ -1549,41 +1549,41 @@
       <c r="AQ12" s="76"/>
     </row>
     <row r="13" spans="1:43" ht="0.45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="85"/>
+      <c r="A13" s="75"/>
       <c r="B13" s="77"/>
       <c r="C13" s="77"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="89"/>
-      <c r="F13" s="89"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="89"/>
-      <c r="J13" s="89"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="89"/>
-      <c r="M13" s="89"/>
-      <c r="N13" s="89"/>
-      <c r="O13" s="89"/>
-      <c r="P13" s="89"/>
-      <c r="Q13" s="89"/>
-      <c r="R13" s="89"/>
-      <c r="S13" s="89"/>
-      <c r="T13" s="89"/>
-      <c r="U13" s="89"/>
-      <c r="V13" s="89"/>
-      <c r="W13" s="89"/>
-      <c r="X13" s="89"/>
-      <c r="Y13" s="89"/>
-      <c r="Z13" s="89"/>
-      <c r="AA13" s="89"/>
-      <c r="AB13" s="89"/>
-      <c r="AC13" s="89"/>
-      <c r="AD13" s="89"/>
-      <c r="AE13" s="89"/>
-      <c r="AF13" s="89"/>
-      <c r="AG13" s="89"/>
-      <c r="AH13" s="89"/>
-      <c r="AI13" s="89"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="81"/>
+      <c r="N13" s="81"/>
+      <c r="O13" s="81"/>
+      <c r="P13" s="81"/>
+      <c r="Q13" s="81"/>
+      <c r="R13" s="81"/>
+      <c r="S13" s="81"/>
+      <c r="T13" s="81"/>
+      <c r="U13" s="81"/>
+      <c r="V13" s="81"/>
+      <c r="W13" s="81"/>
+      <c r="X13" s="81"/>
+      <c r="Y13" s="81"/>
+      <c r="Z13" s="81"/>
+      <c r="AA13" s="81"/>
+      <c r="AB13" s="81"/>
+      <c r="AC13" s="81"/>
+      <c r="AD13" s="81"/>
+      <c r="AE13" s="81"/>
+      <c r="AF13" s="81"/>
+      <c r="AG13" s="81"/>
+      <c r="AH13" s="81"/>
+      <c r="AI13" s="81"/>
       <c r="AJ13" s="77"/>
       <c r="AK13" s="77"/>
       <c r="AL13" s="77"/>
@@ -1594,41 +1594,41 @@
       <c r="AQ13" s="77"/>
     </row>
     <row r="14" spans="1:43" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="85"/>
+      <c r="A14" s="75"/>
       <c r="B14" s="77"/>
       <c r="C14" s="77"/>
-      <c r="D14" s="87"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="89"/>
-      <c r="I14" s="89"/>
-      <c r="J14" s="89"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="89"/>
-      <c r="M14" s="89"/>
-      <c r="N14" s="89"/>
-      <c r="O14" s="89"/>
-      <c r="P14" s="89"/>
-      <c r="Q14" s="89"/>
-      <c r="R14" s="89"/>
-      <c r="S14" s="89"/>
-      <c r="T14" s="89"/>
-      <c r="U14" s="89"/>
-      <c r="V14" s="89"/>
-      <c r="W14" s="89"/>
-      <c r="X14" s="89"/>
-      <c r="Y14" s="89"/>
-      <c r="Z14" s="89"/>
-      <c r="AA14" s="89"/>
-      <c r="AB14" s="89"/>
-      <c r="AC14" s="89"/>
-      <c r="AD14" s="89"/>
-      <c r="AE14" s="89"/>
-      <c r="AF14" s="89"/>
-      <c r="AG14" s="89"/>
-      <c r="AH14" s="89"/>
-      <c r="AI14" s="89"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="81"/>
+      <c r="N14" s="81"/>
+      <c r="O14" s="81"/>
+      <c r="P14" s="81"/>
+      <c r="Q14" s="81"/>
+      <c r="R14" s="81"/>
+      <c r="S14" s="81"/>
+      <c r="T14" s="81"/>
+      <c r="U14" s="81"/>
+      <c r="V14" s="81"/>
+      <c r="W14" s="81"/>
+      <c r="X14" s="81"/>
+      <c r="Y14" s="81"/>
+      <c r="Z14" s="81"/>
+      <c r="AA14" s="81"/>
+      <c r="AB14" s="81"/>
+      <c r="AC14" s="81"/>
+      <c r="AD14" s="81"/>
+      <c r="AE14" s="81"/>
+      <c r="AF14" s="81"/>
+      <c r="AG14" s="81"/>
+      <c r="AH14" s="81"/>
+      <c r="AI14" s="81"/>
       <c r="AJ14" s="77"/>
       <c r="AK14" s="77"/>
       <c r="AL14" s="77"/>
@@ -1639,41 +1639,41 @@
       <c r="AQ14" s="77"/>
     </row>
     <row r="15" spans="1:43" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="85"/>
+      <c r="A15" s="75"/>
       <c r="B15" s="77"/>
       <c r="C15" s="77"/>
-      <c r="D15" s="87"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="89"/>
-      <c r="H15" s="89"/>
-      <c r="I15" s="89"/>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="89"/>
-      <c r="M15" s="89"/>
-      <c r="N15" s="89"/>
-      <c r="O15" s="89"/>
-      <c r="P15" s="89"/>
-      <c r="Q15" s="89"/>
-      <c r="R15" s="89"/>
-      <c r="S15" s="89"/>
-      <c r="T15" s="89"/>
-      <c r="U15" s="89"/>
-      <c r="V15" s="89"/>
-      <c r="W15" s="89"/>
-      <c r="X15" s="89"/>
-      <c r="Y15" s="89"/>
-      <c r="Z15" s="89"/>
-      <c r="AA15" s="89"/>
-      <c r="AB15" s="89"/>
-      <c r="AC15" s="89"/>
-      <c r="AD15" s="89"/>
-      <c r="AE15" s="89"/>
-      <c r="AF15" s="89"/>
-      <c r="AG15" s="89"/>
-      <c r="AH15" s="89"/>
-      <c r="AI15" s="89"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="81"/>
+      <c r="K15" s="81"/>
+      <c r="L15" s="81"/>
+      <c r="M15" s="81"/>
+      <c r="N15" s="81"/>
+      <c r="O15" s="81"/>
+      <c r="P15" s="81"/>
+      <c r="Q15" s="81"/>
+      <c r="R15" s="81"/>
+      <c r="S15" s="81"/>
+      <c r="T15" s="81"/>
+      <c r="U15" s="81"/>
+      <c r="V15" s="81"/>
+      <c r="W15" s="81"/>
+      <c r="X15" s="81"/>
+      <c r="Y15" s="81"/>
+      <c r="Z15" s="81"/>
+      <c r="AA15" s="81"/>
+      <c r="AB15" s="81"/>
+      <c r="AC15" s="81"/>
+      <c r="AD15" s="81"/>
+      <c r="AE15" s="81"/>
+      <c r="AF15" s="81"/>
+      <c r="AG15" s="81"/>
+      <c r="AH15" s="81"/>
+      <c r="AI15" s="81"/>
       <c r="AJ15" s="77"/>
       <c r="AK15" s="77"/>
       <c r="AL15" s="77"/>
@@ -1684,10 +1684,10 @@
       <c r="AQ15" s="77"/>
     </row>
     <row r="16" spans="1:43" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="85"/>
+      <c r="A16" s="75"/>
       <c r="B16" s="77"/>
       <c r="C16" s="77"/>
-      <c r="D16" s="87"/>
+      <c r="D16" s="79"/>
       <c r="E16" s="48">
         <v>1</v>
       </c>
@@ -1845,10 +1845,7 @@
       <c r="AJ17" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="AK17" s="117">
-        <f>INT(DATEDIF($AF$9,$AI$9,"d")+ 1)-COUNTIF(E17:AI17,"В")-AM17-AO17-AQ17</f>
-        <v>31</v>
-      </c>
+      <c r="AK17" s="117"/>
       <c r="AL17" s="66"/>
       <c r="AM17" s="66"/>
       <c r="AN17" s="66"/>
@@ -1940,15 +1937,15 @@
       <c r="AI19" s="41"/>
       <c r="AJ19" s="41"/>
       <c r="AK19" s="41"/>
-      <c r="AL19" s="78">
+      <c r="AL19" s="82">
         <f>Y9</f>
         <v>44090</v>
       </c>
-      <c r="AM19" s="78"/>
-      <c r="AN19" s="78"/>
-      <c r="AO19" s="78"/>
-      <c r="AP19" s="78"/>
-      <c r="AQ19" s="78"/>
+      <c r="AM19" s="82"/>
+      <c r="AN19" s="82"/>
+      <c r="AO19" s="82"/>
+      <c r="AP19" s="82"/>
+      <c r="AQ19" s="82"/>
       <c r="AS19" s="60"/>
       <c r="AT19" s="41"/>
       <c r="AU19" s="41"/>
@@ -1984,39 +1981,39 @@
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20" s="42"/>
-      <c r="M20" s="69" t="s">
+      <c r="M20" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
-      <c r="P20" s="69"/>
+      <c r="N20" s="72"/>
+      <c r="O20" s="72"/>
+      <c r="P20" s="72"/>
       <c r="Q20" s="41"/>
       <c r="R20" s="52"/>
       <c r="S20" s="52"/>
       <c r="T20" s="52"/>
-      <c r="U20" s="79" t="s">
+      <c r="U20" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="V20" s="79"/>
-      <c r="W20" s="79"/>
-      <c r="X20" s="79"/>
-      <c r="Y20" s="79"/>
+      <c r="V20" s="83"/>
+      <c r="W20" s="83"/>
+      <c r="X20" s="83"/>
+      <c r="Y20" s="83"/>
       <c r="Z20" s="59"/>
-      <c r="AA20" s="79" t="s">
+      <c r="AA20" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="AB20" s="79"/>
-      <c r="AC20" s="79"/>
-      <c r="AD20" s="79"/>
-      <c r="AE20" s="79"/>
+      <c r="AB20" s="83"/>
+      <c r="AC20" s="83"/>
+      <c r="AD20" s="83"/>
+      <c r="AE20" s="83"/>
       <c r="AF20" s="47"/>
       <c r="AG20" s="47"/>
       <c r="AH20" s="47"/>
-      <c r="AI20" s="80" t="s">
+      <c r="AI20" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="AJ20" s="80"/>
-      <c r="AK20" s="80"/>
+      <c r="AJ20" s="84"/>
+      <c r="AK20" s="84"/>
       <c r="AL20" s="60"/>
       <c r="AM20" s="60"/>
       <c r="AN20" s="60"/>
@@ -2081,9 +2078,9 @@
       <c r="AF21" s="51"/>
       <c r="AG21" s="51"/>
       <c r="AH21" s="51"/>
-      <c r="AI21" s="81"/>
-      <c r="AJ21" s="81"/>
-      <c r="AK21" s="81"/>
+      <c r="AI21" s="85"/>
+      <c r="AJ21" s="85"/>
+      <c r="AK21" s="85"/>
       <c r="AL21" s="41"/>
       <c r="AM21" s="41"/>
       <c r="AN21" s="41"/>
@@ -2387,28 +2384,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="AN1:AP1"/>
-    <mergeCell ref="AJ2:AM2"/>
-    <mergeCell ref="AN2:AP2"/>
-    <mergeCell ref="C3:AI3"/>
-    <mergeCell ref="AJ3:AL3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AN4:AP4"/>
-    <mergeCell ref="C5:AL5"/>
-    <mergeCell ref="T7:X8"/>
-    <mergeCell ref="Y7:AC8"/>
-    <mergeCell ref="AF7:AK7"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:B16"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="D12:D16"/>
-    <mergeCell ref="E12:AI15"/>
-    <mergeCell ref="AN12:AQ15"/>
-    <mergeCell ref="AL19:AQ19"/>
-    <mergeCell ref="U20:Y20"/>
-    <mergeCell ref="AA20:AE20"/>
-    <mergeCell ref="AI20:AK21"/>
-    <mergeCell ref="AJ12:AM15"/>
     <mergeCell ref="M20:P20"/>
     <mergeCell ref="AF8:AH8"/>
     <mergeCell ref="AF9:AH9"/>
@@ -2417,6 +2392,28 @@
     <mergeCell ref="B9:S9"/>
     <mergeCell ref="T9:X9"/>
     <mergeCell ref="Y9:AC9"/>
+    <mergeCell ref="AN12:AQ15"/>
+    <mergeCell ref="AL19:AQ19"/>
+    <mergeCell ref="U20:Y20"/>
+    <mergeCell ref="AA20:AE20"/>
+    <mergeCell ref="AI20:AK21"/>
+    <mergeCell ref="AJ12:AM15"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="D12:D16"/>
+    <mergeCell ref="E12:AI15"/>
+    <mergeCell ref="AN4:AP4"/>
+    <mergeCell ref="C5:AL5"/>
+    <mergeCell ref="T7:X8"/>
+    <mergeCell ref="Y7:AC8"/>
+    <mergeCell ref="AF7:AK7"/>
+    <mergeCell ref="AN1:AP1"/>
+    <mergeCell ref="AJ2:AM2"/>
+    <mergeCell ref="AN2:AP2"/>
+    <mergeCell ref="C3:AI3"/>
+    <mergeCell ref="AJ3:AL3"/>
+    <mergeCell ref="AN3:AP3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2450,123 +2447,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AO1" s="106" t="s">
+      <c r="AO1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="AP1" s="106"/>
-      <c r="AQ1" s="106"/>
+      <c r="AP1" s="97"/>
+      <c r="AQ1" s="97"/>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="AK2" s="107" t="s">
+      <c r="AK2" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="AL2" s="107"/>
-      <c r="AM2" s="107"/>
-      <c r="AN2" s="107"/>
-      <c r="AO2" s="106">
+      <c r="AL2" s="94"/>
+      <c r="AM2" s="94"/>
+      <c r="AN2" s="94"/>
+      <c r="AO2" s="97">
         <v>301008</v>
       </c>
-      <c r="AP2" s="106"/>
-      <c r="AQ2" s="106"/>
+      <c r="AP2" s="97"/>
+      <c r="AQ2" s="97"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="107"/>
-      <c r="D3" s="116" t="s">
+      <c r="C3" s="94"/>
+      <c r="D3" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="116"/>
-      <c r="F3" s="116"/>
-      <c r="G3" s="116"/>
-      <c r="H3" s="116"/>
-      <c r="I3" s="116"/>
-      <c r="J3" s="116"/>
-      <c r="K3" s="116"/>
-      <c r="L3" s="116"/>
-      <c r="M3" s="116"/>
-      <c r="N3" s="116"/>
-      <c r="O3" s="116"/>
-      <c r="P3" s="116"/>
-      <c r="Q3" s="116"/>
-      <c r="R3" s="116"/>
-      <c r="S3" s="116"/>
-      <c r="T3" s="116"/>
-      <c r="U3" s="116"/>
-      <c r="V3" s="116"/>
-      <c r="W3" s="116"/>
-      <c r="X3" s="116"/>
-      <c r="Y3" s="116"/>
-      <c r="Z3" s="116"/>
-      <c r="AA3" s="116"/>
-      <c r="AB3" s="116"/>
-      <c r="AC3" s="116"/>
-      <c r="AD3" s="116"/>
-      <c r="AE3" s="116"/>
-      <c r="AF3" s="116"/>
-      <c r="AG3" s="116"/>
-      <c r="AH3" s="116"/>
-      <c r="AI3" s="116"/>
-      <c r="AJ3" s="116"/>
-      <c r="AK3" s="114" t="s">
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
+      <c r="R3" s="95"/>
+      <c r="S3" s="95"/>
+      <c r="T3" s="95"/>
+      <c r="U3" s="95"/>
+      <c r="V3" s="95"/>
+      <c r="W3" s="95"/>
+      <c r="X3" s="95"/>
+      <c r="Y3" s="95"/>
+      <c r="Z3" s="95"/>
+      <c r="AA3" s="95"/>
+      <c r="AB3" s="95"/>
+      <c r="AC3" s="95"/>
+      <c r="AD3" s="95"/>
+      <c r="AE3" s="95"/>
+      <c r="AF3" s="95"/>
+      <c r="AG3" s="95"/>
+      <c r="AH3" s="95"/>
+      <c r="AI3" s="95"/>
+      <c r="AJ3" s="95"/>
+      <c r="AK3" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="AL3" s="114"/>
-      <c r="AM3" s="114"/>
-      <c r="AO3" s="106"/>
-      <c r="AP3" s="106"/>
-      <c r="AQ3" s="106"/>
+      <c r="AL3" s="96"/>
+      <c r="AM3" s="96"/>
+      <c r="AO3" s="97"/>
+      <c r="AP3" s="97"/>
+      <c r="AQ3" s="97"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
       <c r="AN4" s="1"/>
-      <c r="AO4" s="106"/>
-      <c r="AP4" s="106"/>
-      <c r="AQ4" s="106"/>
+      <c r="AO4" s="97"/>
+      <c r="AP4" s="97"/>
+      <c r="AQ4" s="97"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B5" s="114" t="s">
+      <c r="B5" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="114"/>
-      <c r="D5" s="116" t="s">
+      <c r="C5" s="96"/>
+      <c r="D5" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="116"/>
-      <c r="K5" s="116"/>
-      <c r="L5" s="116"/>
-      <c r="M5" s="116"/>
-      <c r="N5" s="116"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="116"/>
-      <c r="R5" s="116"/>
-      <c r="S5" s="116"/>
-      <c r="T5" s="116"/>
-      <c r="U5" s="116"/>
-      <c r="V5" s="116"/>
-      <c r="W5" s="116"/>
-      <c r="X5" s="116"/>
-      <c r="Y5" s="116"/>
-      <c r="Z5" s="116"/>
-      <c r="AA5" s="116"/>
-      <c r="AB5" s="116"/>
-      <c r="AC5" s="116"/>
-      <c r="AD5" s="116"/>
-      <c r="AE5" s="116"/>
-      <c r="AF5" s="116"/>
-      <c r="AG5" s="116"/>
-      <c r="AH5" s="116"/>
-      <c r="AI5" s="116"/>
-      <c r="AJ5" s="116"/>
-      <c r="AK5" s="116"/>
-      <c r="AL5" s="116"/>
-      <c r="AM5" s="116"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="95"/>
+      <c r="M5" s="95"/>
+      <c r="N5" s="95"/>
+      <c r="O5" s="95"/>
+      <c r="P5" s="95"/>
+      <c r="Q5" s="95"/>
+      <c r="R5" s="95"/>
+      <c r="S5" s="95"/>
+      <c r="T5" s="95"/>
+      <c r="U5" s="95"/>
+      <c r="V5" s="95"/>
+      <c r="W5" s="95"/>
+      <c r="X5" s="95"/>
+      <c r="Y5" s="95"/>
+      <c r="Z5" s="95"/>
+      <c r="AA5" s="95"/>
+      <c r="AB5" s="95"/>
+      <c r="AC5" s="95"/>
+      <c r="AD5" s="95"/>
+      <c r="AE5" s="95"/>
+      <c r="AF5" s="95"/>
+      <c r="AG5" s="95"/>
+      <c r="AH5" s="95"/>
+      <c r="AI5" s="95"/>
+      <c r="AJ5" s="95"/>
+      <c r="AK5" s="95"/>
+      <c r="AL5" s="95"/>
+      <c r="AM5" s="95"/>
       <c r="AN5" s="1"/>
       <c r="AO5" s="2"/>
       <c r="AP5" s="2"/>
@@ -2574,301 +2571,301 @@
     </row>
     <row r="6" spans="1:44" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U7" s="115" t="s">
+      <c r="U7" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="V7" s="115"/>
-      <c r="W7" s="115"/>
-      <c r="X7" s="115"/>
-      <c r="Y7" s="115"/>
-      <c r="Z7" s="115" t="s">
+      <c r="V7" s="98"/>
+      <c r="W7" s="98"/>
+      <c r="X7" s="98"/>
+      <c r="Y7" s="98"/>
+      <c r="Z7" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="AA7" s="115"/>
-      <c r="AB7" s="115"/>
-      <c r="AC7" s="115"/>
-      <c r="AD7" s="115"/>
-      <c r="AG7" s="115" t="s">
+      <c r="AA7" s="98"/>
+      <c r="AB7" s="98"/>
+      <c r="AC7" s="98"/>
+      <c r="AD7" s="98"/>
+      <c r="AG7" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="AH7" s="115"/>
-      <c r="AI7" s="115"/>
-      <c r="AJ7" s="115"/>
-      <c r="AK7" s="115"/>
-      <c r="AL7" s="115"/>
+      <c r="AH7" s="98"/>
+      <c r="AI7" s="98"/>
+      <c r="AJ7" s="98"/>
+      <c r="AK7" s="98"/>
+      <c r="AL7" s="98"/>
     </row>
     <row r="8" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="U8" s="115"/>
-      <c r="V8" s="115"/>
-      <c r="W8" s="115"/>
-      <c r="X8" s="115"/>
-      <c r="Y8" s="115"/>
-      <c r="Z8" s="115"/>
-      <c r="AA8" s="115"/>
-      <c r="AB8" s="115"/>
-      <c r="AC8" s="115"/>
-      <c r="AD8" s="115"/>
-      <c r="AG8" s="115" t="s">
+      <c r="U8" s="98"/>
+      <c r="V8" s="98"/>
+      <c r="W8" s="98"/>
+      <c r="X8" s="98"/>
+      <c r="Y8" s="98"/>
+      <c r="Z8" s="98"/>
+      <c r="AA8" s="98"/>
+      <c r="AB8" s="98"/>
+      <c r="AC8" s="98"/>
+      <c r="AD8" s="98"/>
+      <c r="AG8" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="AH8" s="115"/>
-      <c r="AI8" s="115"/>
-      <c r="AJ8" s="115"/>
-      <c r="AK8" s="115" t="s">
+      <c r="AH8" s="98"/>
+      <c r="AI8" s="98"/>
+      <c r="AJ8" s="98"/>
+      <c r="AK8" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="AL8" s="115"/>
+      <c r="AL8" s="98"/>
     </row>
     <row r="9" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="101" t="s">
+      <c r="C9" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="101"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
-      <c r="M9" s="101"/>
-      <c r="N9" s="101"/>
-      <c r="O9" s="101"/>
-      <c r="P9" s="101"/>
-      <c r="Q9" s="101"/>
-      <c r="R9" s="101"/>
-      <c r="S9" s="101"/>
-      <c r="T9" s="101"/>
-      <c r="U9" s="102"/>
-      <c r="V9" s="102"/>
-      <c r="W9" s="102"/>
-      <c r="X9" s="102"/>
-      <c r="Y9" s="102"/>
-      <c r="Z9" s="103">
+      <c r="D9" s="111"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="111"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="111"/>
+      <c r="K9" s="111"/>
+      <c r="L9" s="111"/>
+      <c r="M9" s="111"/>
+      <c r="N9" s="111"/>
+      <c r="O9" s="111"/>
+      <c r="P9" s="111"/>
+      <c r="Q9" s="111"/>
+      <c r="R9" s="111"/>
+      <c r="S9" s="111"/>
+      <c r="T9" s="111"/>
+      <c r="U9" s="112"/>
+      <c r="V9" s="112"/>
+      <c r="W9" s="112"/>
+      <c r="X9" s="112"/>
+      <c r="Y9" s="112"/>
+      <c r="Z9" s="113">
         <v>41260</v>
       </c>
-      <c r="AA9" s="103"/>
-      <c r="AB9" s="103"/>
-      <c r="AC9" s="103"/>
-      <c r="AD9" s="103"/>
-      <c r="AG9" s="103">
+      <c r="AA9" s="113"/>
+      <c r="AB9" s="113"/>
+      <c r="AC9" s="113"/>
+      <c r="AD9" s="113"/>
+      <c r="AG9" s="113">
         <v>41244</v>
       </c>
-      <c r="AH9" s="103"/>
-      <c r="AI9" s="103"/>
-      <c r="AJ9" s="103"/>
-      <c r="AK9" s="103">
+      <c r="AH9" s="113"/>
+      <c r="AI9" s="113"/>
+      <c r="AJ9" s="113"/>
+      <c r="AK9" s="113">
         <v>41274</v>
       </c>
-      <c r="AL9" s="103"/>
+      <c r="AL9" s="113"/>
     </row>
     <row r="12" spans="1:44" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="108" t="s">
+      <c r="A12" s="99" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="104" t="s">
+      <c r="C12" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="105" t="s">
+      <c r="D12" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="112" t="s">
+      <c r="E12" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="104" t="s">
+      <c r="F12" s="101" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="104"/>
-      <c r="H12" s="104"/>
-      <c r="I12" s="104"/>
-      <c r="J12" s="104"/>
-      <c r="K12" s="104"/>
-      <c r="L12" s="104"/>
-      <c r="M12" s="104"/>
-      <c r="N12" s="104"/>
-      <c r="O12" s="104"/>
-      <c r="P12" s="104"/>
-      <c r="Q12" s="104"/>
-      <c r="R12" s="104"/>
-      <c r="S12" s="104"/>
-      <c r="T12" s="104"/>
-      <c r="U12" s="104"/>
-      <c r="V12" s="104"/>
-      <c r="W12" s="104"/>
-      <c r="X12" s="104"/>
-      <c r="Y12" s="104"/>
-      <c r="Z12" s="104"/>
-      <c r="AA12" s="104"/>
-      <c r="AB12" s="104"/>
-      <c r="AC12" s="104"/>
-      <c r="AD12" s="104"/>
-      <c r="AE12" s="104"/>
-      <c r="AF12" s="104"/>
-      <c r="AG12" s="104"/>
-      <c r="AH12" s="104"/>
-      <c r="AI12" s="104"/>
-      <c r="AJ12" s="104"/>
-      <c r="AK12" s="105" t="s">
+      <c r="G12" s="101"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="101"/>
+      <c r="J12" s="101"/>
+      <c r="K12" s="101"/>
+      <c r="L12" s="101"/>
+      <c r="M12" s="101"/>
+      <c r="N12" s="101"/>
+      <c r="O12" s="101"/>
+      <c r="P12" s="101"/>
+      <c r="Q12" s="101"/>
+      <c r="R12" s="101"/>
+      <c r="S12" s="101"/>
+      <c r="T12" s="101"/>
+      <c r="U12" s="101"/>
+      <c r="V12" s="101"/>
+      <c r="W12" s="101"/>
+      <c r="X12" s="101"/>
+      <c r="Y12" s="101"/>
+      <c r="Z12" s="101"/>
+      <c r="AA12" s="101"/>
+      <c r="AB12" s="101"/>
+      <c r="AC12" s="101"/>
+      <c r="AD12" s="101"/>
+      <c r="AE12" s="101"/>
+      <c r="AF12" s="101"/>
+      <c r="AG12" s="101"/>
+      <c r="AH12" s="101"/>
+      <c r="AI12" s="101"/>
+      <c r="AJ12" s="101"/>
+      <c r="AK12" s="103" t="s">
         <v>18</v>
       </c>
-      <c r="AL12" s="105"/>
-      <c r="AM12" s="105"/>
-      <c r="AN12" s="105"/>
-      <c r="AO12" s="105" t="s">
+      <c r="AL12" s="103"/>
+      <c r="AM12" s="103"/>
+      <c r="AN12" s="103"/>
+      <c r="AO12" s="103" t="s">
         <v>19</v>
       </c>
-      <c r="AP12" s="105"/>
-      <c r="AQ12" s="105"/>
-      <c r="AR12" s="105"/>
+      <c r="AP12" s="103"/>
+      <c r="AQ12" s="103"/>
+      <c r="AR12" s="103"/>
     </row>
     <row r="13" spans="1:44" ht="0.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="108"/>
-      <c r="B13" s="108"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="112"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="104"/>
-      <c r="H13" s="104"/>
-      <c r="I13" s="104"/>
-      <c r="J13" s="104"/>
-      <c r="K13" s="104"/>
-      <c r="L13" s="104"/>
-      <c r="M13" s="104"/>
-      <c r="N13" s="104"/>
-      <c r="O13" s="104"/>
-      <c r="P13" s="104"/>
-      <c r="Q13" s="104"/>
-      <c r="R13" s="104"/>
-      <c r="S13" s="104"/>
-      <c r="T13" s="104"/>
-      <c r="U13" s="104"/>
-      <c r="V13" s="104"/>
-      <c r="W13" s="104"/>
-      <c r="X13" s="104"/>
-      <c r="Y13" s="104"/>
-      <c r="Z13" s="104"/>
-      <c r="AA13" s="104"/>
-      <c r="AB13" s="104"/>
-      <c r="AC13" s="104"/>
-      <c r="AD13" s="104"/>
-      <c r="AE13" s="104"/>
-      <c r="AF13" s="104"/>
-      <c r="AG13" s="104"/>
-      <c r="AH13" s="104"/>
-      <c r="AI13" s="104"/>
-      <c r="AJ13" s="104"/>
-      <c r="AK13" s="105"/>
-      <c r="AL13" s="105"/>
-      <c r="AM13" s="105"/>
-      <c r="AN13" s="105"/>
-      <c r="AO13" s="105"/>
-      <c r="AP13" s="105"/>
-      <c r="AQ13" s="105"/>
-      <c r="AR13" s="105"/>
+      <c r="A13" s="99"/>
+      <c r="B13" s="99"/>
+      <c r="C13" s="101"/>
+      <c r="D13" s="103"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="101"/>
+      <c r="G13" s="101"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="101"/>
+      <c r="J13" s="101"/>
+      <c r="K13" s="101"/>
+      <c r="L13" s="101"/>
+      <c r="M13" s="101"/>
+      <c r="N13" s="101"/>
+      <c r="O13" s="101"/>
+      <c r="P13" s="101"/>
+      <c r="Q13" s="101"/>
+      <c r="R13" s="101"/>
+      <c r="S13" s="101"/>
+      <c r="T13" s="101"/>
+      <c r="U13" s="101"/>
+      <c r="V13" s="101"/>
+      <c r="W13" s="101"/>
+      <c r="X13" s="101"/>
+      <c r="Y13" s="101"/>
+      <c r="Z13" s="101"/>
+      <c r="AA13" s="101"/>
+      <c r="AB13" s="101"/>
+      <c r="AC13" s="101"/>
+      <c r="AD13" s="101"/>
+      <c r="AE13" s="101"/>
+      <c r="AF13" s="101"/>
+      <c r="AG13" s="101"/>
+      <c r="AH13" s="101"/>
+      <c r="AI13" s="101"/>
+      <c r="AJ13" s="101"/>
+      <c r="AK13" s="103"/>
+      <c r="AL13" s="103"/>
+      <c r="AM13" s="103"/>
+      <c r="AN13" s="103"/>
+      <c r="AO13" s="103"/>
+      <c r="AP13" s="103"/>
+      <c r="AQ13" s="103"/>
+      <c r="AR13" s="103"/>
     </row>
     <row r="14" spans="1:44" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="108"/>
-      <c r="B14" s="108"/>
-      <c r="C14" s="104"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="112"/>
-      <c r="F14" s="104"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="104"/>
-      <c r="I14" s="104"/>
-      <c r="J14" s="104"/>
-      <c r="K14" s="104"/>
-      <c r="L14" s="104"/>
-      <c r="M14" s="104"/>
-      <c r="N14" s="104"/>
-      <c r="O14" s="104"/>
-      <c r="P14" s="104"/>
-      <c r="Q14" s="104"/>
-      <c r="R14" s="104"/>
-      <c r="S14" s="104"/>
-      <c r="T14" s="104"/>
-      <c r="U14" s="104"/>
-      <c r="V14" s="104"/>
-      <c r="W14" s="104"/>
-      <c r="X14" s="104"/>
-      <c r="Y14" s="104"/>
-      <c r="Z14" s="104"/>
-      <c r="AA14" s="104"/>
-      <c r="AB14" s="104"/>
-      <c r="AC14" s="104"/>
-      <c r="AD14" s="104"/>
-      <c r="AE14" s="104"/>
-      <c r="AF14" s="104"/>
-      <c r="AG14" s="104"/>
-      <c r="AH14" s="104"/>
-      <c r="AI14" s="104"/>
-      <c r="AJ14" s="104"/>
-      <c r="AK14" s="105"/>
-      <c r="AL14" s="105"/>
-      <c r="AM14" s="105"/>
-      <c r="AN14" s="105"/>
-      <c r="AO14" s="105"/>
-      <c r="AP14" s="105"/>
-      <c r="AQ14" s="105"/>
-      <c r="AR14" s="105"/>
+      <c r="A14" s="99"/>
+      <c r="B14" s="99"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="105"/>
+      <c r="F14" s="101"/>
+      <c r="G14" s="101"/>
+      <c r="H14" s="101"/>
+      <c r="I14" s="101"/>
+      <c r="J14" s="101"/>
+      <c r="K14" s="101"/>
+      <c r="L14" s="101"/>
+      <c r="M14" s="101"/>
+      <c r="N14" s="101"/>
+      <c r="O14" s="101"/>
+      <c r="P14" s="101"/>
+      <c r="Q14" s="101"/>
+      <c r="R14" s="101"/>
+      <c r="S14" s="101"/>
+      <c r="T14" s="101"/>
+      <c r="U14" s="101"/>
+      <c r="V14" s="101"/>
+      <c r="W14" s="101"/>
+      <c r="X14" s="101"/>
+      <c r="Y14" s="101"/>
+      <c r="Z14" s="101"/>
+      <c r="AA14" s="101"/>
+      <c r="AB14" s="101"/>
+      <c r="AC14" s="101"/>
+      <c r="AD14" s="101"/>
+      <c r="AE14" s="101"/>
+      <c r="AF14" s="101"/>
+      <c r="AG14" s="101"/>
+      <c r="AH14" s="101"/>
+      <c r="AI14" s="101"/>
+      <c r="AJ14" s="101"/>
+      <c r="AK14" s="103"/>
+      <c r="AL14" s="103"/>
+      <c r="AM14" s="103"/>
+      <c r="AN14" s="103"/>
+      <c r="AO14" s="103"/>
+      <c r="AP14" s="103"/>
+      <c r="AQ14" s="103"/>
+      <c r="AR14" s="103"/>
     </row>
     <row r="15" spans="1:44" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="108"/>
-      <c r="B15" s="108"/>
-      <c r="C15" s="104"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="112"/>
-      <c r="F15" s="104"/>
-      <c r="G15" s="104"/>
-      <c r="H15" s="104"/>
-      <c r="I15" s="104"/>
-      <c r="J15" s="104"/>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
-      <c r="M15" s="104"/>
-      <c r="N15" s="104"/>
-      <c r="O15" s="104"/>
-      <c r="P15" s="104"/>
-      <c r="Q15" s="104"/>
-      <c r="R15" s="104"/>
-      <c r="S15" s="104"/>
-      <c r="T15" s="104"/>
-      <c r="U15" s="104"/>
-      <c r="V15" s="104"/>
-      <c r="W15" s="104"/>
-      <c r="X15" s="104"/>
-      <c r="Y15" s="104"/>
-      <c r="Z15" s="104"/>
-      <c r="AA15" s="104"/>
-      <c r="AB15" s="104"/>
-      <c r="AC15" s="104"/>
-      <c r="AD15" s="104"/>
-      <c r="AE15" s="104"/>
-      <c r="AF15" s="104"/>
-      <c r="AG15" s="104"/>
-      <c r="AH15" s="104"/>
-      <c r="AI15" s="104"/>
-      <c r="AJ15" s="104"/>
-      <c r="AK15" s="105"/>
-      <c r="AL15" s="105"/>
-      <c r="AM15" s="105"/>
-      <c r="AN15" s="105"/>
-      <c r="AO15" s="105"/>
-      <c r="AP15" s="105"/>
-      <c r="AQ15" s="105"/>
-      <c r="AR15" s="105"/>
+      <c r="A15" s="99"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="101"/>
+      <c r="D15" s="103"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="101"/>
+      <c r="G15" s="101"/>
+      <c r="H15" s="101"/>
+      <c r="I15" s="101"/>
+      <c r="J15" s="101"/>
+      <c r="K15" s="101"/>
+      <c r="L15" s="101"/>
+      <c r="M15" s="101"/>
+      <c r="N15" s="101"/>
+      <c r="O15" s="101"/>
+      <c r="P15" s="101"/>
+      <c r="Q15" s="101"/>
+      <c r="R15" s="101"/>
+      <c r="S15" s="101"/>
+      <c r="T15" s="101"/>
+      <c r="U15" s="101"/>
+      <c r="V15" s="101"/>
+      <c r="W15" s="101"/>
+      <c r="X15" s="101"/>
+      <c r="Y15" s="101"/>
+      <c r="Z15" s="101"/>
+      <c r="AA15" s="101"/>
+      <c r="AB15" s="101"/>
+      <c r="AC15" s="101"/>
+      <c r="AD15" s="101"/>
+      <c r="AE15" s="101"/>
+      <c r="AF15" s="101"/>
+      <c r="AG15" s="101"/>
+      <c r="AH15" s="101"/>
+      <c r="AI15" s="101"/>
+      <c r="AJ15" s="101"/>
+      <c r="AK15" s="103"/>
+      <c r="AL15" s="103"/>
+      <c r="AM15" s="103"/>
+      <c r="AN15" s="103"/>
+      <c r="AO15" s="103"/>
+      <c r="AP15" s="103"/>
+      <c r="AQ15" s="103"/>
+      <c r="AR15" s="103"/>
     </row>
     <row r="16" spans="1:44" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="109"/>
-      <c r="B16" s="109"/>
-      <c r="C16" s="110"/>
-      <c r="D16" s="111"/>
-      <c r="E16" s="113"/>
+      <c r="A16" s="100"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="106"/>
       <c r="F16" s="20">
         <v>1</v>
       </c>
@@ -3637,13 +3634,13 @@
       <c r="N30" s="7"/>
       <c r="O30" s="7"/>
       <c r="P30" s="8"/>
-      <c r="Q30" s="97" t="s">
+      <c r="Q30" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="R30" s="97"/>
-      <c r="S30" s="97"/>
-      <c r="T30" s="97"/>
-      <c r="U30" s="97"/>
+      <c r="R30" s="110"/>
+      <c r="S30" s="110"/>
+      <c r="T30" s="110"/>
+      <c r="U30" s="110"/>
       <c r="V30" s="4"/>
       <c r="W30" s="4"/>
       <c r="X30" s="4"/>
@@ -3669,41 +3666,41 @@
       <c r="AR30" s="4"/>
     </row>
     <row r="31" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="97" t="s">
+      <c r="A31" s="110" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="97"/>
+      <c r="B31" s="110"/>
       <c r="C31" s="16" t="s">
         <v>38</v>
       </c>
       <c r="D31" s="56"/>
       <c r="E31" s="57"/>
-      <c r="F31" s="98" t="s">
+      <c r="F31" s="116" t="s">
         <v>39</v>
       </c>
-      <c r="G31" s="98"/>
-      <c r="H31" s="98"/>
-      <c r="I31" s="98"/>
-      <c r="J31" s="98"/>
+      <c r="G31" s="116"/>
+      <c r="H31" s="116"/>
+      <c r="I31" s="116"/>
+      <c r="J31" s="116"/>
       <c r="K31" s="10"/>
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
       <c r="O31" s="7"/>
       <c r="P31" s="8"/>
-      <c r="Q31" s="97"/>
-      <c r="R31" s="97"/>
-      <c r="S31" s="97"/>
-      <c r="T31" s="97"/>
-      <c r="U31" s="97"/>
+      <c r="Q31" s="110"/>
+      <c r="R31" s="110"/>
+      <c r="S31" s="110"/>
+      <c r="T31" s="110"/>
+      <c r="U31" s="110"/>
       <c r="V31" s="57"/>
-      <c r="W31" s="99" t="s">
+      <c r="W31" s="107" t="s">
         <v>40</v>
       </c>
-      <c r="X31" s="99"/>
-      <c r="Y31" s="99"/>
-      <c r="Z31" s="99"/>
-      <c r="AA31" s="99"/>
+      <c r="X31" s="107"/>
+      <c r="Y31" s="107"/>
+      <c r="Z31" s="107"/>
+      <c r="AA31" s="107"/>
       <c r="AB31" s="57"/>
       <c r="AC31" s="56"/>
       <c r="AD31" s="56"/>
@@ -3711,30 +3708,30 @@
       <c r="AF31" s="56"/>
       <c r="AG31" s="56"/>
       <c r="AH31" s="57"/>
-      <c r="AI31" s="99" t="s">
+      <c r="AI31" s="107" t="s">
         <v>41</v>
       </c>
-      <c r="AJ31" s="99"/>
-      <c r="AK31" s="99"/>
-      <c r="AL31" s="99"/>
+      <c r="AJ31" s="107"/>
+      <c r="AK31" s="107"/>
+      <c r="AL31" s="107"/>
       <c r="AM31" s="57"/>
       <c r="AN31" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="AO31" s="100" t="s">
+      <c r="AO31" s="108" t="s">
         <v>43</v>
       </c>
-      <c r="AP31" s="100"/>
-      <c r="AQ31" s="100"/>
+      <c r="AP31" s="108"/>
+      <c r="AQ31" s="108"/>
       <c r="AR31" s="57" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:44" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="94" t="s">
+      <c r="A32" s="109" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="94"/>
+      <c r="B32" s="109"/>
       <c r="C32" s="9" t="s">
         <v>25</v>
       </c>
@@ -3742,47 +3739,47 @@
         <v>26</v>
       </c>
       <c r="E32" s="57"/>
-      <c r="F32" s="95" t="s">
+      <c r="F32" s="114" t="s">
         <v>27</v>
       </c>
-      <c r="G32" s="95"/>
-      <c r="H32" s="95"/>
-      <c r="I32" s="95"/>
-      <c r="J32" s="95"/>
+      <c r="G32" s="114"/>
+      <c r="H32" s="114"/>
+      <c r="I32" s="114"/>
+      <c r="J32" s="114"/>
       <c r="K32" s="10"/>
       <c r="L32" s="12"/>
       <c r="M32" s="13"/>
       <c r="N32" s="13"/>
       <c r="O32" s="13"/>
       <c r="P32" s="57"/>
-      <c r="Q32" s="97"/>
-      <c r="R32" s="97"/>
-      <c r="S32" s="97"/>
-      <c r="T32" s="97"/>
-      <c r="U32" s="97"/>
+      <c r="Q32" s="110"/>
+      <c r="R32" s="110"/>
+      <c r="S32" s="110"/>
+      <c r="T32" s="110"/>
+      <c r="U32" s="110"/>
       <c r="V32" s="57"/>
-      <c r="W32" s="96" t="s">
+      <c r="W32" s="115" t="s">
         <v>25</v>
       </c>
-      <c r="X32" s="96"/>
-      <c r="Y32" s="96"/>
-      <c r="Z32" s="96"/>
-      <c r="AA32" s="96"/>
+      <c r="X32" s="115"/>
+      <c r="Y32" s="115"/>
+      <c r="Z32" s="115"/>
+      <c r="AA32" s="115"/>
       <c r="AB32" s="57"/>
-      <c r="AC32" s="94" t="s">
+      <c r="AC32" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="AD32" s="94"/>
-      <c r="AE32" s="94"/>
-      <c r="AF32" s="94"/>
-      <c r="AG32" s="94"/>
+      <c r="AD32" s="109"/>
+      <c r="AE32" s="109"/>
+      <c r="AF32" s="109"/>
+      <c r="AG32" s="109"/>
       <c r="AH32" s="4"/>
-      <c r="AI32" s="97" t="s">
+      <c r="AI32" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="AJ32" s="97"/>
-      <c r="AK32" s="97"/>
-      <c r="AL32" s="97"/>
+      <c r="AJ32" s="110"/>
+      <c r="AK32" s="110"/>
+      <c r="AL32" s="110"/>
       <c r="AM32" s="57"/>
       <c r="AN32" s="57"/>
       <c r="AO32" s="57"/>
@@ -3796,11 +3793,11 @@
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
       <c r="E33" s="14"/>
-      <c r="F33" s="95"/>
-      <c r="G33" s="95"/>
-      <c r="H33" s="95"/>
-      <c r="I33" s="95"/>
-      <c r="J33" s="95"/>
+      <c r="F33" s="114"/>
+      <c r="G33" s="114"/>
+      <c r="H33" s="114"/>
+      <c r="I33" s="114"/>
+      <c r="J33" s="114"/>
       <c r="K33" s="14"/>
       <c r="L33" s="14"/>
       <c r="M33" s="14"/>
@@ -3825,10 +3822,10 @@
       <c r="AF33" s="15"/>
       <c r="AG33" s="15"/>
       <c r="AH33" s="15"/>
-      <c r="AI33" s="97"/>
-      <c r="AJ33" s="97"/>
-      <c r="AK33" s="97"/>
-      <c r="AL33" s="97"/>
+      <c r="AI33" s="110"/>
+      <c r="AJ33" s="110"/>
+      <c r="AK33" s="110"/>
+      <c r="AL33" s="110"/>
       <c r="AM33" s="14"/>
       <c r="AN33" s="14"/>
       <c r="AO33" s="14"/>
@@ -4177,11 +4174,24 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="39">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:AJ3"/>
-    <mergeCell ref="AK3:AM3"/>
-    <mergeCell ref="AO3:AQ3"/>
-    <mergeCell ref="AG7:AL7"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="F32:J33"/>
+    <mergeCell ref="W32:AA32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="F31:J31"/>
+    <mergeCell ref="W31:AA31"/>
+    <mergeCell ref="AI31:AL31"/>
+    <mergeCell ref="AO31:AQ31"/>
+    <mergeCell ref="AC32:AG32"/>
+    <mergeCell ref="AI32:AL33"/>
+    <mergeCell ref="C9:T9"/>
+    <mergeCell ref="U9:Y9"/>
+    <mergeCell ref="Z9:AD9"/>
+    <mergeCell ref="AG9:AJ9"/>
+    <mergeCell ref="AK9:AL9"/>
+    <mergeCell ref="F12:AJ15"/>
+    <mergeCell ref="AK12:AN15"/>
+    <mergeCell ref="Q30:U32"/>
     <mergeCell ref="AO1:AQ1"/>
     <mergeCell ref="AK2:AN2"/>
     <mergeCell ref="AO2:AQ2"/>
@@ -4198,24 +4208,11 @@
     <mergeCell ref="D5:AM5"/>
     <mergeCell ref="U7:Y8"/>
     <mergeCell ref="Z7:AD8"/>
-    <mergeCell ref="AI31:AL31"/>
-    <mergeCell ref="AO31:AQ31"/>
-    <mergeCell ref="AC32:AG32"/>
-    <mergeCell ref="AI32:AL33"/>
-    <mergeCell ref="C9:T9"/>
-    <mergeCell ref="U9:Y9"/>
-    <mergeCell ref="Z9:AD9"/>
-    <mergeCell ref="AG9:AJ9"/>
-    <mergeCell ref="AK9:AL9"/>
-    <mergeCell ref="F12:AJ15"/>
-    <mergeCell ref="AK12:AN15"/>
-    <mergeCell ref="Q30:U32"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="F32:J33"/>
-    <mergeCell ref="W32:AA32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="F31:J31"/>
-    <mergeCell ref="W31:AA31"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:AJ3"/>
+    <mergeCell ref="AK3:AM3"/>
+    <mergeCell ref="AO3:AQ3"/>
+    <mergeCell ref="AG7:AL7"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78749999999999998" right="0.39374999999999999" top="1.1812499999999999" bottom="0.98402777777777772" header="0.51180555555555551" footer="0.51180555555555551"/>

</xml_diff>